<commit_message>
add up to 15 levels
</commit_message>
<xml_diff>
--- a/levels/level2.xlsx
+++ b/levels/level2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\mobgenerator_weaponswitcher\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other projects\Weapons switcher\mobgenerator_weaponswitcher\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2003BE26-FBB2-45AB-9FEE-D8AA381BA24C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37470" windowHeight="21840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37476" windowHeight="21840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="enemies" sheetId="3" r:id="rId3"/>
     <sheet name="misc" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,20 +438,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -468,12 +467,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -483,20 +482,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -508,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2</v>
       </c>
@@ -520,13 +519,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E3">
         <f>meta!$B$1*ROW()</f>
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -538,7 +537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -550,19 +549,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6">
         <f>meta!$B$1*ROW()</f>
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7">
         <f>meta!$B$1*ROW()</f>
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -577,7 +576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>2</v>
       </c>
@@ -586,19 +585,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10">
         <f>meta!$B$1*ROW()</f>
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11">
         <f>meta!$B$1*ROW()</f>
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>4</v>
       </c>
@@ -610,19 +609,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>meta!$B$1*ROW()</f>
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E14">
         <f>meta!$B$1*ROW()</f>
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -634,13 +633,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16">
         <f>meta!$B$1*ROW()</f>
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>4</v>
       </c>
@@ -649,13 +648,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E18">
         <f>meta!$B$1*ROW()</f>
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>4</v>
       </c>
@@ -667,175 +666,175 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E20">
         <f>meta!$B$1*ROW()</f>
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E21">
         <f>meta!$B$1*ROW()</f>
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E22">
         <f>meta!$B$1*ROW()</f>
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E23">
         <f>meta!$B$1*ROW()</f>
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E24">
         <f>meta!$B$1*ROW()</f>
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E25">
         <f>meta!$B$1*ROW()</f>
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E26">
         <f>meta!$B$1*ROW()</f>
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E27">
         <f>meta!$B$1*ROW()</f>
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E28">
         <f>meta!$B$1*ROW()</f>
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E29">
         <f>meta!$B$1*ROW()</f>
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E30">
         <f>meta!$B$1*ROW()</f>
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31">
         <f>meta!$B$1*ROW()</f>
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E32">
         <f>meta!$B$1*ROW()</f>
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33">
         <f>meta!$B$1*ROW()</f>
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34">
         <f>meta!$B$1*ROW()</f>
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35">
         <f>meta!$B$1*ROW()</f>
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36">
         <f>meta!$B$1*ROW()</f>
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37">
         <f>meta!$B$1*ROW()</f>
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38">
         <f>meta!$B$1*ROW()</f>
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39">
         <f>meta!$B$1*ROW()</f>
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40">
         <f>meta!$B$1*ROW()</f>
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41">
         <f>meta!$B$1*ROW()</f>
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42">
         <f>meta!$B$1*ROW()</f>
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43">
         <f>meta!$B$1*ROW()</f>
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44">
         <f>meta!$B$1*ROW()</f>
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45">
         <f>meta!$B$1*ROW()</f>
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46">
         <f>meta!$B$1*ROW()</f>
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47">
         <f>meta!$B$1*ROW()</f>
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48">
         <f>meta!$B$1*ROW()</f>
         <v>144</v>
@@ -848,28 +847,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="57.88671875" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -889,7 +888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -909,7 +908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -929,7 +928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -949,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -969,7 +968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -992,7 +991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1022,94 +1021,94 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB22E08-D7E6-44F4-914F-485CD0DA319A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.85546875" customWidth="1"/>
+    <col min="1" max="1" width="73.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>

</xml_diff>